<commit_message>
TICKET2383 - Consolidated Reports * Modified excel template Impressions sheet
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3598 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-1.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4605" windowWidth="21840" windowHeight="10800" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="4605" windowWidth="21840" windowHeight="10800" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1797,10 +1797,10 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>8219.2799999999988</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9588.75</c:v>
+                  <c:v>3401.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4150</c:v>
@@ -2370,11 +2370,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="50407680"/>
-        <c:axId val="83761792"/>
+        <c:axId val="128196992"/>
+        <c:axId val="128198528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50407680"/>
+        <c:axId val="128196992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83761792"/>
+        <c:crossAx val="128198528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2410,7 +2410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83761792"/>
+        <c:axId val="128198528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,7 +2438,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50407680"/>
+        <c:crossAx val="128196992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2806,12 +2806,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="83990016"/>
-        <c:axId val="90066944"/>
+        <c:axId val="128207488"/>
+        <c:axId val="128225664"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="83990016"/>
+        <c:axId val="128207488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2829,7 +2829,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="90066944"/>
+        <c:crossAx val="128225664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2837,7 +2837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90066944"/>
+        <c:axId val="128225664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2865,7 +2865,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83990016"/>
+        <c:crossAx val="128207488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3129,12 +3129,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="91599232"/>
-        <c:axId val="91600768"/>
+        <c:axId val="128279680"/>
+        <c:axId val="128281216"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="91599232"/>
+        <c:axId val="128279680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91600768"/>
+        <c:crossAx val="128281216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3170,7 +3170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91600768"/>
+        <c:axId val="128281216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3198,7 +3198,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91599232"/>
+        <c:crossAx val="128279680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3408,22 +3408,22 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>362000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>233000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>249000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42656</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3442,12 +3442,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="29500544"/>
-        <c:axId val="29502080"/>
+        <c:axId val="128293504"/>
+        <c:axId val="128315776"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="29500544"/>
+        <c:axId val="128293504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3475,7 +3475,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29502080"/>
+        <c:crossAx val="128315776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3483,7 +3483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29502080"/>
+        <c:axId val="128315776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3511,7 +3511,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29500544"/>
+        <c:crossAx val="128293504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3685,7 +3685,7 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8250</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4535</c:v>
@@ -3704,11 +3704,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="29547136"/>
-        <c:axId val="30212480"/>
+        <c:axId val="128401792"/>
+        <c:axId val="128403328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="29547136"/>
+        <c:axId val="128401792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,7 +3736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30212480"/>
+        <c:crossAx val="128403328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3744,7 +3744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30212480"/>
+        <c:axId val="128403328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3754,7 +3754,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="29547136"/>
+        <c:crossAx val="128401792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5651,9 +5651,9 @@
       <c r="G8" s="42"/>
       <c r="H8" s="49"/>
       <c r="I8" s="151"/>
-      <c r="J8" s="147">
+      <c r="J8" s="147" t="e">
         <f>'Activity Summary'!I31</f>
-        <v>41408.03</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K8" s="128" t="s">
         <v>169</v>
@@ -5697,9 +5697,9 @@
       <c r="G10" s="42"/>
       <c r="H10" s="49"/>
       <c r="I10" s="151"/>
-      <c r="J10" s="147">
+      <c r="J10" s="147" t="e">
         <f>J8+J9</f>
-        <v>93486.03</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K10" s="128" t="s">
         <v>181</v>
@@ -5720,9 +5720,9 @@
       <c r="G11" s="42"/>
       <c r="H11" s="49"/>
       <c r="I11" s="151"/>
-      <c r="J11" s="144">
+      <c r="J11" s="144" t="e">
         <f>J10/J7</f>
-        <v>9.3486030000000007</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="K11" s="128" t="s">
         <v>140</v>
@@ -7796,35 +7796,35 @@
       </c>
       <c r="B11" s="8">
         <f>Impressions!F8</f>
-        <v>55000</v>
-      </c>
-      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17" t="e">
         <f>C26/5</f>
-        <v>697.47239383853753</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D11" s="8">
         <f>Impressions!F9</f>
-        <v>102000</v>
-      </c>
-      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17" t="e">
         <f>E26/5</f>
-        <v>405.1079124951915</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F11" s="8">
         <f>Impressions!F10</f>
-        <v>315000</v>
-      </c>
-      <c r="G11" s="164">
+        <v>0</v>
+      </c>
+      <c r="G11" s="164" t="e">
         <f>G26/5</f>
-        <v>541.27569366627074</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H11" s="8">
         <f t="shared" ref="H11:I13" si="0">B11+D11+F11</f>
-        <v>472000</v>
-      </c>
-      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17" t="e">
         <f t="shared" si="0"/>
-        <v>1643.8559999999998</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J11" s="18">
         <v>0.1</v>
@@ -7836,11 +7836,11 @@
       </c>
       <c r="B12" s="8">
         <f>0.03*B11</f>
-        <v>1650</v>
+        <v>0</v>
       </c>
       <c r="C12" s="17">
         <f>B12*$J12</f>
-        <v>1237.5</v>
+        <v>0</v>
       </c>
       <c r="D12" s="8">
         <v>907</v>
@@ -7859,11 +7859,11 @@
       </c>
       <c r="H12" s="8">
         <f t="shared" si="0"/>
-        <v>2557</v>
+        <v>907</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" si="0"/>
-        <v>1917.75</v>
+        <v>680.25</v>
       </c>
       <c r="J12" s="18">
         <v>0.75</v>
@@ -7988,24 +7988,24 @@
         <v>150</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="23">
+      <c r="C16" s="23" t="e">
         <f>SUM(C11:C15)</f>
-        <v>5164.9723938385378</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="23">
+      <c r="E16" s="23" t="e">
         <f>SUM(E11:E15)</f>
-        <v>2575.3579124951916</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F16" s="8"/>
-      <c r="G16" s="23">
+      <c r="G16" s="23" t="e">
         <f>SUM(G11:G15)</f>
-        <v>541.27569366627074</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="23">
+      <c r="I16" s="23" t="e">
         <f>SUM(I11:I15)</f>
-        <v>8281.6059999999998</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -8066,21 +8066,21 @@
         <v>80</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="28">
+      <c r="C19" s="28" t="e">
         <f>C16+C18</f>
-        <v>9584.9723938385378</v>
-      </c>
-      <c r="E19" s="28">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="28" t="e">
         <f>E16+E18</f>
-        <v>5695.3579124951921</v>
-      </c>
-      <c r="G19" s="28">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G19" s="28" t="e">
         <f>G16+G18</f>
-        <v>16141.27569366627</v>
-      </c>
-      <c r="I19" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I19" s="39" t="e">
         <f>I16+I18</f>
-        <v>31421.606</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -8175,35 +8175,35 @@
       </c>
       <c r="B26" s="8">
         <f>Impressions!N8</f>
-        <v>405900</v>
-      </c>
-      <c r="C26" s="17">
+        <v>0</v>
+      </c>
+      <c r="C26" s="17" t="e">
         <f>Impressions!O8</f>
-        <v>3487.3619691926874</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D26" s="8">
         <f>Impressions!N9</f>
-        <v>235756</v>
-      </c>
-      <c r="E26" s="17">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17" t="e">
         <f>Impressions!O9</f>
-        <v>2025.5395624759576</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F26" s="8">
         <f>Impressions!N10</f>
-        <v>315000</v>
-      </c>
-      <c r="G26" s="17">
+        <v>0</v>
+      </c>
+      <c r="G26" s="17" t="e">
         <f>Impressions!O10</f>
-        <v>2706.3784683313538</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H26" s="8">
         <f t="shared" ref="H26:I30" si="3">B26+D26+F26</f>
-        <v>956656</v>
-      </c>
-      <c r="I26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="17" t="e">
         <f t="shared" si="3"/>
-        <v>8219.2799999999988</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J26" s="18">
         <f>J11</f>
@@ -8216,11 +8216,11 @@
       </c>
       <c r="B27" s="8">
         <f>B12*5</f>
-        <v>8250</v>
+        <v>0</v>
       </c>
       <c r="C27" s="17">
         <f>B27*$J27</f>
-        <v>6187.5</v>
+        <v>0</v>
       </c>
       <c r="D27" s="8">
         <f>D12*5</f>
@@ -8239,11 +8239,11 @@
       </c>
       <c r="H27" s="8">
         <f t="shared" si="3"/>
-        <v>12785</v>
+        <v>4535</v>
       </c>
       <c r="I27" s="17">
         <f t="shared" si="3"/>
-        <v>9588.75</v>
+        <v>3401.25</v>
       </c>
       <c r="J27" s="18">
         <f>J12</f>
@@ -8381,24 +8381,24 @@
         <v>150</v>
       </c>
       <c r="B31" s="8"/>
-      <c r="C31" s="23">
+      <c r="C31" s="23" t="e">
         <f>SUM(C26:C30)</f>
-        <v>25824.861969192687</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="23">
+      <c r="E31" s="23" t="e">
         <f>SUM(E26:E30)</f>
-        <v>12876.789562475959</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="F31" s="8"/>
-      <c r="G31" s="23">
+      <c r="G31" s="23" t="e">
         <f>SUM(G26:G30)</f>
-        <v>2706.3784683313538</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="H31" s="8"/>
-      <c r="I31" s="23">
+      <c r="I31" s="23" t="e">
         <f>SUM(I26:I30)</f>
-        <v>41408.03</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="J31" s="18"/>
     </row>
@@ -8466,21 +8466,21 @@
         <v>80</v>
       </c>
       <c r="B34" s="8"/>
-      <c r="C34" s="28">
+      <c r="C34" s="28" t="e">
         <f>C31+C33</f>
-        <v>49744.861969192687</v>
-      </c>
-      <c r="E34" s="28">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E34" s="28" t="e">
         <f>E31+E33</f>
-        <v>25434.789562475959</v>
-      </c>
-      <c r="G34" s="28">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34" s="28" t="e">
         <f>G31+G33</f>
-        <v>18306.378468331353</v>
-      </c>
-      <c r="I34" s="39">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="39" t="e">
         <f>I31+I33</f>
-        <v>93486.03</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -8903,15 +8903,15 @@
       </c>
       <c r="B72" s="9">
         <f>B26</f>
-        <v>405900</v>
+        <v>0</v>
       </c>
       <c r="C72" s="9">
         <f t="shared" si="4"/>
-        <v>235756</v>
+        <v>0</v>
       </c>
       <c r="D72" s="9">
         <f t="shared" si="5"/>
-        <v>315000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
@@ -8921,7 +8921,7 @@
       </c>
       <c r="B73" s="9">
         <f>B27</f>
-        <v>8250</v>
+        <v>0</v>
       </c>
       <c r="C73" s="9">
         <f t="shared" si="4"/>
@@ -9847,8 +9847,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9986,53 +9986,18 @@
       <c r="A7" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="33">
-        <v>40554</v>
-      </c>
-      <c r="C7" s="33">
-        <f>B7+30</f>
-        <v>40584</v>
-      </c>
-      <c r="D7" s="33">
-        <f t="shared" ref="D7:M7" si="0">C7+30</f>
-        <v>40614</v>
-      </c>
-      <c r="E7" s="33">
-        <f t="shared" si="0"/>
-        <v>40644</v>
-      </c>
-      <c r="F7" s="33">
-        <f t="shared" si="0"/>
-        <v>40674</v>
-      </c>
-      <c r="G7" s="33">
-        <f t="shared" si="0"/>
-        <v>40704</v>
-      </c>
-      <c r="H7" s="33">
-        <f t="shared" si="0"/>
-        <v>40734</v>
-      </c>
-      <c r="I7" s="33">
-        <f t="shared" si="0"/>
-        <v>40764</v>
-      </c>
-      <c r="J7" s="33">
-        <f t="shared" si="0"/>
-        <v>40794</v>
-      </c>
-      <c r="K7" s="33">
-        <f t="shared" si="0"/>
-        <v>40824</v>
-      </c>
-      <c r="L7" s="33">
-        <f t="shared" si="0"/>
-        <v>40854</v>
-      </c>
-      <c r="M7" s="33">
-        <f t="shared" si="0"/>
-        <v>40884</v>
-      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
       <c r="N7" s="120" t="s">
         <v>46</v>
       </c>
@@ -10045,22 +10010,11 @@
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="8">
-        <v>51000</v>
-      </c>
-      <c r="C8" s="8">
-        <v>48000</v>
-      </c>
-      <c r="D8" s="8">
-        <v>71000</v>
-      </c>
-      <c r="E8" s="8">
-        <f>159000+E23</f>
-        <v>180900</v>
-      </c>
-      <c r="F8" s="8">
-        <v>55000</v>
-      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -10070,11 +10024,11 @@
       <c r="M8" s="8"/>
       <c r="N8" s="62">
         <f>SUM(B8:M8)</f>
-        <v>405900</v>
-      </c>
-      <c r="O8" s="28">
+        <v>0</v>
+      </c>
+      <c r="O8" s="28" t="e">
         <f>N8/N$12*O$27</f>
-        <v>3487.3619691926874</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P8" s="42"/>
     </row>
@@ -10082,24 +10036,11 @@
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="8">
-        <f>31000+B23</f>
-        <v>31000</v>
-      </c>
-      <c r="C9" s="8">
-        <f>31000+C23</f>
-        <v>40756</v>
-      </c>
-      <c r="D9" s="8">
-        <v>31000</v>
-      </c>
-      <c r="E9" s="8">
-        <f>31000</f>
-        <v>31000</v>
-      </c>
-      <c r="F9" s="8">
-        <v>102000</v>
-      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -10109,11 +10050,11 @@
       <c r="M9" s="8"/>
       <c r="N9" s="62">
         <f>SUM(B9:M9)</f>
-        <v>235756</v>
-      </c>
-      <c r="O9" s="28">
+        <v>0</v>
+      </c>
+      <c r="O9" s="28" t="e">
         <f>N9/N$12*O$27</f>
-        <v>2025.5395624759576</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P9" s="42"/>
     </row>
@@ -10125,9 +10066,7 @@
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="8">
-        <v>315000</v>
-      </c>
+      <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
@@ -10137,11 +10076,11 @@
       <c r="M10" s="8"/>
       <c r="N10" s="62">
         <f>SUM(B10:M10)</f>
-        <v>315000</v>
-      </c>
-      <c r="O10" s="28">
+        <v>0</v>
+      </c>
+      <c r="O10" s="28" t="e">
         <f>N10/N$12*O$27</f>
-        <v>2706.3784683313538</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P10" s="42"/>
     </row>
@@ -10166,60 +10105,60 @@
         <v>45</v>
       </c>
       <c r="B12" s="25">
-        <f t="shared" ref="B12:M12" si="1">SUM(B8:B10)</f>
-        <v>82000</v>
+        <f t="shared" ref="B12:M12" si="0">SUM(B8:B10)</f>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
-        <f t="shared" si="1"/>
-        <v>88756</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D12" s="25">
-        <f t="shared" si="1"/>
-        <v>102000</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="E12" s="25">
-        <f t="shared" si="1"/>
-        <v>211900</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="F12" s="25">
-        <f t="shared" si="1"/>
-        <v>472000</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M12" s="25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N12" s="63">
         <f>SUM(B12:M12)</f>
-        <v>956656</v>
-      </c>
-      <c r="O12" s="41">
+        <v>0</v>
+      </c>
+      <c r="O12" s="41" t="e">
         <f>SUM(O8:O10)</f>
-        <v>8219.2799999999988</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P12" s="42"/>
     </row>
@@ -10325,43 +10264,43 @@
         <v>40584</v>
       </c>
       <c r="D18" s="33">
-        <f t="shared" ref="D18:M18" si="2">C18+30</f>
+        <f t="shared" ref="D18:M18" si="1">C18+30</f>
         <v>40614</v>
       </c>
       <c r="E18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40644</v>
       </c>
       <c r="F18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40674</v>
       </c>
       <c r="G18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40704</v>
       </c>
       <c r="H18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40734</v>
       </c>
       <c r="I18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40764</v>
       </c>
       <c r="J18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40794</v>
       </c>
       <c r="K18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40824</v>
       </c>
       <c r="L18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40854</v>
       </c>
       <c r="M18" s="33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40884</v>
       </c>
       <c r="N18" s="120" t="s">
@@ -10378,21 +10317,11 @@
       <c r="A19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="8">
-        <v>49000</v>
-      </c>
-      <c r="C19" s="8">
-        <v>55000</v>
-      </c>
-      <c r="D19" s="8">
-        <v>68000</v>
-      </c>
-      <c r="E19" s="8">
-        <v>52000</v>
-      </c>
-      <c r="F19" s="8">
-        <v>138000</v>
-      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
@@ -10401,12 +10330,12 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="62">
-        <f t="shared" ref="N19:N25" si="3">SUM(B19:M19)</f>
-        <v>362000</v>
+        <f t="shared" ref="N19:N25" si="2">SUM(B19:M19)</f>
+        <v>0</v>
       </c>
       <c r="O19" s="28">
         <f>(N19/1000)*P19</f>
-        <v>4344</v>
+        <v>0</v>
       </c>
       <c r="P19" s="17">
         <v>12</v>
@@ -10416,21 +10345,11 @@
       <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="8">
-        <v>10000</v>
-      </c>
-      <c r="C20" s="8">
-        <v>12000</v>
-      </c>
-      <c r="D20" s="8">
-        <v>13000</v>
-      </c>
-      <c r="E20" s="8">
-        <v>14000</v>
-      </c>
-      <c r="F20" s="8">
-        <v>21000</v>
-      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
@@ -10439,12 +10358,12 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="62">
-        <f t="shared" si="3"/>
-        <v>70000</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="O20" s="28">
-        <f t="shared" ref="O20:O25" si="4">(N20/1000)*P20</f>
-        <v>700</v>
+        <f t="shared" ref="O20:O25" si="3">(N20/1000)*P20</f>
+        <v>0</v>
       </c>
       <c r="P20" s="17">
         <v>10</v>
@@ -10454,21 +10373,11 @@
       <c r="A21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="8">
-        <v>23000</v>
-      </c>
-      <c r="C21" s="8">
-        <v>12000</v>
-      </c>
-      <c r="D21" s="8">
-        <v>21000</v>
-      </c>
-      <c r="E21" s="8">
-        <v>24000</v>
-      </c>
-      <c r="F21" s="8">
-        <v>153000</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
@@ -10477,12 +10386,12 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="28">
         <f t="shared" si="3"/>
-        <v>233000</v>
-      </c>
-      <c r="O21" s="28">
-        <f t="shared" si="4"/>
-        <v>1864</v>
+        <v>0</v>
       </c>
       <c r="P21" s="17">
         <v>8</v>
@@ -10492,21 +10401,11 @@
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="8">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8">
-        <v>0</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0</v>
-      </c>
-      <c r="E22" s="8">
-        <v>100000</v>
-      </c>
-      <c r="F22" s="8">
-        <v>149000</v>
-      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
@@ -10515,12 +10414,12 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="28">
         <f t="shared" si="3"/>
-        <v>249000</v>
-      </c>
-      <c r="O22" s="28">
-        <f t="shared" si="4"/>
-        <v>498</v>
+        <v>0</v>
       </c>
       <c r="P22" s="17">
         <v>2</v>
@@ -10531,16 +10430,10 @@
         <v>73</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="8">
-        <v>9756</v>
-      </c>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="8">
-        <v>21900</v>
-      </c>
-      <c r="F23" s="8">
-        <v>11000</v>
-      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -10549,12 +10442,12 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="28">
         <f t="shared" si="3"/>
-        <v>42656</v>
-      </c>
-      <c r="O23" s="28">
-        <f t="shared" si="4"/>
-        <v>213.28</v>
+        <v>0</v>
       </c>
       <c r="P23" s="17">
         <v>5</v>
@@ -10564,14 +10457,10 @@
       <c r="A24" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
+      <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="8">
-        <v>50000</v>
-      </c>
+      <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -10581,12 +10470,12 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="28">
         <f t="shared" si="3"/>
-        <v>50000</v>
-      </c>
-      <c r="O24" s="28">
-        <f t="shared" si="4"/>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="P24" s="17">
         <v>12</v>
@@ -10609,11 +10498,11 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="28">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="28">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P25" s="17">
@@ -10642,59 +10531,59 @@
       </c>
       <c r="B27" s="26">
         <f>SUM(B19:B25)</f>
-        <v>82000</v>
+        <v>0</v>
       </c>
       <c r="C27" s="26">
-        <f t="shared" ref="C27:M27" si="5">SUM(C19:C25)</f>
-        <v>88756</v>
+        <f t="shared" ref="C27:M27" si="4">SUM(C19:C25)</f>
+        <v>0</v>
       </c>
       <c r="D27" s="26">
-        <f t="shared" si="5"/>
-        <v>102000</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E27" s="26">
-        <f t="shared" si="5"/>
-        <v>261900</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="F27" s="26">
-        <f t="shared" si="5"/>
-        <v>472000</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="G27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N27" s="63">
         <f>SUM(B27:M27)</f>
-        <v>1006656</v>
+        <v>0</v>
       </c>
       <c r="O27" s="41">
         <f>SUM(O19:O25)</f>
-        <v>8219.2799999999988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -12302,7 +12191,7 @@
   </sheetPr>
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TICKET2383 - Consolidated Reports * Updated excel template
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@3602 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-1.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4605" windowWidth="21840" windowHeight="10800" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="4605" windowWidth="21840" windowHeight="10800" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="187">
   <si>
     <t>calls</t>
   </si>
@@ -496,15 +496,9 @@
     <t>Client Dashboard - Year to Date Results</t>
   </si>
   <si>
-    <t>The Superior Hotel, London</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
-    <t>Jan - May 2011</t>
-  </si>
-  <si>
     <t>Agreement Start Date</t>
   </si>
   <si>
@@ -572,9 +566,6 @@
   </si>
   <si>
     <t>Email Address / Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jan 1, 2011 - May 31, 2011</t>
   </si>
   <si>
     <t>Marketing Value (YTD)</t>
@@ -1535,6 +1526,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -1812,7 +1804,7 @@
                   <c:v>10500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52078</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2348,13 +2340,13 @@
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2370,11 +2362,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="128196992"/>
-        <c:axId val="128198528"/>
+        <c:axId val="74948992"/>
+        <c:axId val="74950528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128196992"/>
+        <c:axId val="74948992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128198528"/>
+        <c:crossAx val="74950528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2410,7 +2402,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128198528"/>
+        <c:axId val="74950528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,7 +2430,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128196992"/>
+        <c:crossAx val="74948992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2806,12 +2798,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="128207488"/>
-        <c:axId val="128225664"/>
+        <c:axId val="74963584"/>
+        <c:axId val="75444608"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="128207488"/>
+        <c:axId val="74963584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2829,7 +2821,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128225664"/>
+        <c:crossAx val="75444608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2837,7 +2829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128225664"/>
+        <c:axId val="75444608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2865,7 +2857,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128207488"/>
+        <c:crossAx val="74963584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2942,6 +2934,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3107,13 +3100,13 @@
                 <c:formatCode>_("$"* #,##0_);_("$"* \(#,##0\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23920</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12558</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15600</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3129,12 +3122,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="128279680"/>
-        <c:axId val="128281216"/>
+        <c:axId val="75474048"/>
+        <c:axId val="75475584"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="128279680"/>
+        <c:axId val="75474048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128281216"/>
+        <c:crossAx val="75475584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3170,7 +3163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128281216"/>
+        <c:axId val="75475584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3198,7 +3191,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128279680"/>
+        <c:crossAx val="75474048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3442,12 +3435,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="128293504"/>
-        <c:axId val="128315776"/>
+        <c:axId val="75774592"/>
+        <c:axId val="75776384"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="128293504"/>
+        <c:axId val="75774592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3475,7 +3468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128315776"/>
+        <c:crossAx val="75776384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -3483,7 +3476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128315776"/>
+        <c:axId val="75776384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3511,7 +3504,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="128293504"/>
+        <c:crossAx val="75774592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3704,11 +3697,11 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="128401792"/>
-        <c:axId val="128403328"/>
+        <c:axId val="75790592"/>
+        <c:axId val="75497472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128401792"/>
+        <c:axId val="75790592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3736,7 +3729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="128403328"/>
+        <c:crossAx val="75497472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3744,7 +3737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128403328"/>
+        <c:axId val="75497472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3754,7 +3747,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128401792"/>
+        <c:crossAx val="75790592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4232,7 +4225,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -5485,8 +5478,8 @@
   </sheetPr>
   <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5571,9 +5564,7 @@
       <c r="G4" s="42"/>
       <c r="H4" s="49"/>
       <c r="I4" s="151"/>
-      <c r="J4" s="159" t="s">
-        <v>142</v>
-      </c>
+      <c r="J4" s="159"/>
       <c r="K4" s="50"/>
       <c r="L4" s="50"/>
       <c r="M4" s="50"/>
@@ -5591,9 +5582,7 @@
       <c r="G5" s="42"/>
       <c r="H5" s="49"/>
       <c r="I5" s="151"/>
-      <c r="J5" s="146" t="s">
-        <v>168</v>
-      </c>
+      <c r="J5" s="146"/>
       <c r="K5" s="127"/>
       <c r="L5" s="47"/>
       <c r="M5" s="49"/>
@@ -5629,11 +5618,9 @@
       <c r="G7" s="42"/>
       <c r="H7" s="49"/>
       <c r="I7" s="151"/>
-      <c r="J7" s="147">
-        <v>10000</v>
-      </c>
+      <c r="J7" s="147"/>
       <c r="K7" s="128" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L7" s="49"/>
       <c r="M7" s="49"/>
@@ -5656,7 +5643,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K8" s="128" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L8" s="49"/>
       <c r="M8" s="49"/>
@@ -5676,10 +5663,10 @@
       <c r="I9" s="151"/>
       <c r="J9" s="147">
         <f>Bookings!H22</f>
-        <v>52078</v>
+        <v>0</v>
       </c>
       <c r="K9" s="128" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L9" s="49"/>
       <c r="M9" s="49"/>
@@ -5702,7 +5689,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="128" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L10" s="49"/>
       <c r="M10" s="49"/>
@@ -7580,7 +7567,7 @@
       <c r="K114" s="42"/>
       <c r="L114" s="42"/>
       <c r="O114" s="142" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="P114" s="42"/>
     </row>
@@ -7624,7 +7611,7 @@
   <dimension ref="A1:Q77"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7642,7 +7629,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -7665,9 +7652,9 @@
       <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="136" t="str">
+      <c r="A3" s="136">
         <f>Dashboard!$J$4</f>
-        <v>The Superior Hotel, London</v>
+        <v>0</v>
       </c>
       <c r="B3" s="51"/>
       <c r="C3" s="51"/>
@@ -7680,10 +7667,10 @@
     </row>
     <row r="4" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="161" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="49"/>
       <c r="D4" s="53"/>
@@ -7696,10 +7683,10 @@
     <row r="5" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="162">
         <f>Dashboard!J7</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" s="49"/>
       <c r="D5" s="53"/>
@@ -7711,10 +7698,10 @@
     </row>
     <row r="6" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="161" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B6" s="57" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="53"/>
@@ -7726,7 +7713,7 @@
     </row>
     <row r="7" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="163" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B7" s="59"/>
       <c r="C7" s="54"/>
@@ -7750,7 +7737,7 @@
     </row>
     <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="42"/>
@@ -7762,9 +7749,7 @@
       <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="35">
-        <v>40674</v>
-      </c>
+      <c r="A10" s="35"/>
       <c r="B10" s="37" t="s">
         <v>42</v>
       </c>
@@ -7871,7 +7856,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B13" s="8">
         <v>99</v>
@@ -7985,7 +7970,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="23" t="e">
@@ -8027,35 +8012,35 @@
       </c>
       <c r="B18" s="8">
         <f>Bookings!E7</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C18" s="17">
         <f>Bookings!H7</f>
-        <v>4420</v>
+        <v>0</v>
       </c>
       <c r="D18" s="8">
         <f>Bookings!E8</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E18" s="17">
         <f>Bookings!H8</f>
-        <v>3120</v>
+        <v>0</v>
       </c>
       <c r="F18" s="8">
         <f>Bookings!E9</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G18" s="17">
         <f>Bookings!H9</f>
-        <v>15600</v>
+        <v>0</v>
       </c>
       <c r="H18" s="8">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I18" s="17">
         <f t="shared" si="2"/>
-        <v>23140</v>
+        <v>0</v>
       </c>
       <c r="J18" s="18">
         <v>260</v>
@@ -8141,9 +8126,7 @@
       <c r="I24" s="42"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="36" t="s">
-        <v>144</v>
-      </c>
+      <c r="A25" s="36"/>
       <c r="B25" s="37" t="s">
         <v>42</v>
       </c>
@@ -8252,7 +8235,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B28" s="8">
         <f>B13*5</f>
@@ -8378,7 +8361,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="23" t="e">
@@ -8423,35 +8406,35 @@
       </c>
       <c r="B33" s="8">
         <f>Bookings!E18</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C33" s="17">
         <f>Bookings!H18</f>
-        <v>23920</v>
+        <v>0</v>
       </c>
       <c r="D33" s="8">
         <f>Bookings!E19</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E33" s="17">
         <f>Bookings!H19</f>
-        <v>12558</v>
+        <v>0</v>
       </c>
       <c r="F33" s="8">
         <f>Bookings!E20</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G33" s="17">
         <f>Bookings!H20</f>
-        <v>15600</v>
+        <v>0</v>
       </c>
       <c r="H33" s="8">
         <f>B33+D33+F33</f>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="I33" s="17">
         <f>C33+E33+G33</f>
-        <v>52078</v>
+        <v>0</v>
       </c>
       <c r="J33" s="18">
         <f>J18</f>
@@ -8993,15 +8976,15 @@
       </c>
       <c r="B77" s="9">
         <f>B33</f>
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="C77" s="9">
         <f>D33</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D77" s="9">
         <f>F33</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9026,7 +9009,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9047,7 +9030,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -9060,9 +9043,9 @@
       <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="137" t="str">
+      <c r="A2" s="137">
         <f>Dashboard!$J$4</f>
-        <v>The Superior Hotel, London</v>
+        <v>0</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -9076,11 +9059,9 @@
     </row>
     <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="138" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" s="139">
-        <v>40664</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B3" s="139"/>
       <c r="C3" s="55"/>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -9115,9 +9096,7 @@
       <c r="J5" s="42"/>
     </row>
     <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="34">
-        <v>40674</v>
-      </c>
+      <c r="A6" s="34"/>
       <c r="B6" s="134" t="s">
         <v>81</v>
       </c>
@@ -9137,117 +9116,86 @@
         <v>83</v>
       </c>
       <c r="H6" s="134" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I6" s="134" t="s">
         <v>84</v>
       </c>
       <c r="J6" s="134" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="30">
-        <v>2</v>
-      </c>
-      <c r="C7" s="30">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8">
-        <v>10</v>
-      </c>
-      <c r="E7" s="8">
-        <v>8</v>
-      </c>
-      <c r="F7" s="8">
-        <v>17</v>
-      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="29">
         <f>37%</f>
         <v>0.37</v>
       </c>
       <c r="H7" s="17">
         <f>F7*260</f>
-        <v>4420</v>
+        <v>0</v>
       </c>
       <c r="I7" s="29">
         <v>0.21</v>
       </c>
       <c r="J7" s="17">
         <f>H7*(1-I7)</f>
-        <v>3491.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="30">
-        <v>1</v>
-      </c>
-      <c r="C8" s="30">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D8" s="8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="8">
-        <v>12</v>
-      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="29">
         <v>0.4</v>
       </c>
       <c r="H8" s="17">
         <f>F8*260</f>
-        <v>3120</v>
+        <v>0</v>
       </c>
       <c r="I8" s="29">
         <v>0.21</v>
       </c>
       <c r="J8" s="17">
         <f>H8*(1-I8)</f>
-        <v>2464.8000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="30">
-        <v>0</v>
-      </c>
-      <c r="C9" s="30">
-        <v>1</v>
-      </c>
-      <c r="D9" s="165">
-        <v>20</v>
-      </c>
-      <c r="E9" s="8">
-        <v>20</v>
-      </c>
-      <c r="F9" s="8">
-        <f>3*E9</f>
-        <v>60</v>
-      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="29">
         <v>0</v>
       </c>
       <c r="H9" s="17">
         <f>F9*260</f>
-        <v>15600</v>
+        <v>0</v>
       </c>
       <c r="I9" s="29">
         <v>0.18</v>
       </c>
       <c r="J9" s="17">
         <f>H9*(1-I9)</f>
-        <v>12792.000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -9268,32 +9216,32 @@
       </c>
       <c r="B11" s="30">
         <f>SUM(B7:B10)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="30">
         <f t="shared" ref="C11:J11" si="0">SUM(C7:C10)</f>
-        <v>4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="D11" s="30"/>
       <c r="E11" s="8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="G11" s="29">
         <v>0.38500000000000001</v>
       </c>
       <c r="H11" s="23">
         <f t="shared" si="0"/>
-        <v>23140</v>
+        <v>0</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="23">
         <f t="shared" si="0"/>
-        <v>18748.600000000002</v>
+        <v>0</v>
       </c>
       <c r="K11" s="18">
         <f>'Activity Summary'!J18</f>
@@ -9306,9 +9254,7 @@
       <c r="I12" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="28">
-        <v>1240</v>
-      </c>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" s="14"/>
@@ -9318,7 +9264,7 @@
       </c>
       <c r="J13" s="28">
         <f>J11-J12</f>
-        <v>17508.600000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -9380,119 +9326,86 @@
         <v>83</v>
       </c>
       <c r="H17" s="134" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="I17" s="134" t="s">
         <v>84</v>
       </c>
       <c r="J17" s="134" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="30">
-        <v>4.3</v>
-      </c>
-      <c r="C18" s="30">
-        <v>1.9</v>
-      </c>
-      <c r="D18" s="8">
-        <v>56</v>
-      </c>
-      <c r="E18" s="8">
-        <v>40</v>
-      </c>
-      <c r="F18" s="8">
-        <f>2.3*E18</f>
-        <v>92</v>
-      </c>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="29">
         <f>37%</f>
         <v>0.37</v>
       </c>
       <c r="H18" s="17">
         <f>F18*260</f>
-        <v>23920</v>
+        <v>0</v>
       </c>
       <c r="I18" s="29">
         <v>0.21</v>
       </c>
       <c r="J18" s="17">
         <f>H18*(1-I18)</f>
-        <v>18896.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="30">
-        <v>1</v>
-      </c>
-      <c r="C19" s="30">
-        <v>0.9</v>
-      </c>
-      <c r="D19" s="8">
-        <v>27</v>
-      </c>
-      <c r="E19" s="8">
-        <v>21</v>
-      </c>
-      <c r="F19" s="8">
-        <f>2.3*E19</f>
-        <v>48.3</v>
-      </c>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="29">
         <v>0.4</v>
       </c>
       <c r="H19" s="17">
         <f>F19*260</f>
-        <v>12558</v>
+        <v>0</v>
       </c>
       <c r="I19" s="29">
         <v>0.21</v>
       </c>
       <c r="J19" s="17">
         <f>H19*(1-I19)</f>
-        <v>9920.82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="30">
-        <v>0</v>
-      </c>
-      <c r="C20" s="30">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8">
-        <v>20</v>
-      </c>
-      <c r="E20" s="8">
-        <v>20</v>
-      </c>
-      <c r="F20" s="8">
-        <f>3*E20</f>
-        <v>60</v>
-      </c>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="29">
         <v>0</v>
       </c>
       <c r="H20" s="17">
         <f>F20*260</f>
-        <v>15600</v>
+        <v>0</v>
       </c>
       <c r="I20" s="29">
         <v>0.18</v>
       </c>
       <c r="J20" s="17">
         <f>H20*(1-I20)</f>
-        <v>12792.000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -9513,32 +9426,32 @@
       </c>
       <c r="B22" s="30">
         <f>SUM(B18:B21)</f>
-        <v>5.3</v>
+        <v>0</v>
       </c>
       <c r="C22" s="30">
         <f>SUM(C18:C21)</f>
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="D22" s="30"/>
       <c r="E22" s="8">
         <f>SUM(E18:E21)</f>
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="F22" s="8">
         <f>SUM(F18:F21)</f>
-        <v>200.3</v>
+        <v>0</v>
       </c>
       <c r="G22" s="29">
         <v>0.38500000000000001</v>
       </c>
       <c r="H22" s="23">
         <f>SUM(H18:H21)</f>
-        <v>52078</v>
+        <v>0</v>
       </c>
       <c r="I22" s="29"/>
       <c r="J22" s="23">
         <f>SUM(J18:J21)</f>
-        <v>41609.620000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -9553,10 +9466,7 @@
       <c r="I23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="J23" s="28">
-        <f>1240*5</f>
-        <v>6200</v>
-      </c>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I24" s="7" t="s">
@@ -9564,7 +9474,7 @@
       </c>
       <c r="J24" s="28">
         <f>J22-J23</f>
-        <v>35409.620000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -9612,7 +9522,7 @@
       <c r="G28" s="42"/>
       <c r="H28" s="42"/>
       <c r="I28" s="166" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J28" s="166"/>
     </row>
@@ -9847,20 +9757,14 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="16" max="16" width="7" customWidth="1"/>
@@ -9869,7 +9773,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -9888,9 +9792,9 @@
       <c r="P1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="135" t="str">
+      <c r="A2" s="135">
         <f>Dashboard!$J$4</f>
-        <v>The Superior Hotel, London</v>
+        <v>0</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -9910,7 +9814,7 @@
     </row>
     <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="106" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B3" s="107"/>
       <c r="C3" s="108"/>
@@ -10257,51 +10161,52 @@
         <v>41</v>
       </c>
       <c r="B18" s="33">
-        <v>40554</v>
+        <f>B7</f>
+        <v>0</v>
       </c>
       <c r="C18" s="33">
-        <f>B18+30</f>
-        <v>40584</v>
+        <f>C7</f>
+        <v>0</v>
       </c>
       <c r="D18" s="33">
-        <f t="shared" ref="D18:M18" si="1">C18+30</f>
-        <v>40614</v>
+        <f>D7</f>
+        <v>0</v>
       </c>
       <c r="E18" s="33">
-        <f t="shared" si="1"/>
-        <v>40644</v>
+        <f>E7</f>
+        <v>0</v>
       </c>
       <c r="F18" s="33">
-        <f t="shared" si="1"/>
-        <v>40674</v>
+        <f>F7</f>
+        <v>0</v>
       </c>
       <c r="G18" s="33">
-        <f t="shared" si="1"/>
-        <v>40704</v>
+        <f>G7</f>
+        <v>0</v>
       </c>
       <c r="H18" s="33">
-        <f t="shared" si="1"/>
-        <v>40734</v>
+        <f>H7</f>
+        <v>0</v>
       </c>
       <c r="I18" s="33">
-        <f t="shared" si="1"/>
-        <v>40764</v>
+        <f>I7</f>
+        <v>0</v>
       </c>
       <c r="J18" s="33">
-        <f t="shared" si="1"/>
-        <v>40794</v>
+        <f>J7</f>
+        <v>0</v>
       </c>
       <c r="K18" s="33">
-        <f t="shared" si="1"/>
-        <v>40824</v>
+        <f>K7</f>
+        <v>0</v>
       </c>
       <c r="L18" s="33">
-        <f t="shared" si="1"/>
-        <v>40854</v>
+        <f>L7</f>
+        <v>0</v>
       </c>
       <c r="M18" s="33">
-        <f t="shared" si="1"/>
-        <v>40884</v>
+        <f>M7</f>
+        <v>0</v>
       </c>
       <c r="N18" s="120" t="s">
         <v>46</v>
@@ -10330,7 +10235,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="62">
-        <f t="shared" ref="N19:N25" si="2">SUM(B19:M19)</f>
+        <f t="shared" ref="N19:N25" si="1">SUM(B19:M19)</f>
         <v>0</v>
       </c>
       <c r="O19" s="28">
@@ -10358,11 +10263,11 @@
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O20" s="28">
-        <f t="shared" ref="O20:O25" si="3">(N20/1000)*P20</f>
+        <f t="shared" ref="O20:O25" si="2">(N20/1000)*P20</f>
         <v>0</v>
       </c>
       <c r="P20" s="17">
@@ -10386,11 +10291,11 @@
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
       <c r="N21" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P21" s="17">
@@ -10414,11 +10319,11 @@
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
       <c r="N22" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O22" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O22" s="28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P22" s="17">
@@ -10442,11 +10347,11 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P23" s="17">
@@ -10470,11 +10375,11 @@
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
       <c r="N24" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P24" s="17">
@@ -10498,11 +10403,11 @@
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
       <c r="N25" s="62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="28">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P25" s="17">
@@ -10534,47 +10439,47 @@
         <v>0</v>
       </c>
       <c r="C27" s="26">
-        <f t="shared" ref="C27:M27" si="4">SUM(C19:C25)</f>
+        <f t="shared" ref="C27:M27" si="3">SUM(C19:C25)</f>
         <v>0</v>
       </c>
       <c r="D27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M27" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N27" s="63">
@@ -11207,11 +11112,11 @@
     <hyperlink ref="N34" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -11222,7 +11127,7 @@
   </sheetPr>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -11237,7 +11142,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -11250,7 +11155,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="131" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -11273,9 +11178,9 @@
       <c r="I3" s="111"/>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="137" t="str">
+      <c r="A4" s="137">
         <f>Dashboard!$J$4</f>
-        <v>The Superior Hotel, London</v>
+        <v>0</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -11287,9 +11192,7 @@
       <c r="I4" s="111"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="160">
-        <v>40664</v>
-      </c>
+      <c r="A5" s="160"/>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
       <c r="D5" s="89"/>
@@ -11338,7 +11241,7 @@
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="132" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B9" s="132">
         <v>32</v>
@@ -11353,7 +11256,7 @@
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="110" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="110">
         <v>178</v>
@@ -12191,13 +12094,13 @@
   </sheetPr>
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" style="14" bestFit="1" customWidth="1"/>
@@ -12223,7 +12126,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="26.25" x14ac:dyDescent="0.2">
       <c r="A1" s="104" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="49"/>
@@ -12249,7 +12152,7 @@
     </row>
     <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="131" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -12300,9 +12203,9 @@
       <c r="V3" s="42"/>
     </row>
     <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="137" t="str">
+      <c r="A4" s="137">
         <f>Dashboard!$J$4</f>
-        <v>The Superior Hotel, London</v>
+        <v>0</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -12327,9 +12230,7 @@
       <c r="V4" s="42"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="105">
-        <v>40664</v>
-      </c>
+      <c r="A5" s="105"/>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
       <c r="D5" s="89"/>
@@ -12440,7 +12341,7 @@
         <v>48</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>57</v>
@@ -12458,7 +12359,7 @@
         <v>68</v>
       </c>
       <c r="I9" s="70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J9" s="79" t="s">
         <v>56</v>
@@ -16308,7 +16209,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="167" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B1" s="167"/>
       <c r="C1" s="45"/>
@@ -16328,10 +16229,10 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="145" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B4" s="140" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C4" s="140" t="s">
         <v>32</v>
@@ -16342,10 +16243,10 @@
     </row>
     <row r="5" spans="1:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="90" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="124" t="s">
         <v>39</v>
@@ -16357,13 +16258,13 @@
         <v>33</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6" s="124" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
@@ -16374,7 +16275,7 @@
         <v>34</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" s="124">
         <v>1</v>
@@ -16386,10 +16287,10 @@
     </row>
     <row r="8" spans="1:7" ht="53.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C8" s="124">
         <v>5</v>
@@ -16401,10 +16302,10 @@
     </row>
     <row r="9" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" s="94" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="124">
         <v>10</v>
@@ -16419,7 +16320,7 @@
         <v>35</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="124">
         <v>15</v>
@@ -16434,13 +16335,13 @@
         <v>36</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C11" s="125" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="99" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>

</xml_diff>